<commit_message>
modif format tableaux pour garder la config des platines
</commit_message>
<xml_diff>
--- a/moveset.xlsx
+++ b/moveset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\OneDrive\Documents\Stage ENSTA\FromLabViewToPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEEF9A98-460D-4926-9EF2-1DFAF6EAA250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417137D3-2A75-473A-8235-1F5480F6561E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0F119DA3-7AB5-48FC-9F97-FDAC8791B065}"/>
   </bookViews>
@@ -34,9 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -388,51 +394,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96BDDDF-FD70-4764-99C5-5E0AE548BBD0}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
     </row>

</xml_diff>